<commit_message>
Up sbs 7b 13b
</commit_message>
<xml_diff>
--- a/sbs/gusev_7b_ru_alpaca_lora_gusev_13b_ru_alpaca_lora.xlsx
+++ b/sbs/gusev_7b_ru_alpaca_lora_gusev_13b_ru_alpaca_lora.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkuk/proj/rulm-sbs/sbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA897C-791F-4840-A58A-F59B9C50A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2906756-661A-BE49-9282-20283AE6AE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$55</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1520,10 +1523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1601,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1656,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1703,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1737,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1754,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -1805,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="256" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1839,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -1873,7 +1877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>88</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>92</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -1958,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>100</v>
       </c>
@@ -1975,7 +1979,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>104</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
@@ -2009,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>116</v>
       </c>
@@ -2043,7 +2047,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
@@ -2060,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>124</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="304" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>128</v>
       </c>
@@ -2090,8 +2094,11 @@
       <c r="D33" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="E33" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>132</v>
       </c>
@@ -2104,8 +2111,11 @@
       <c r="D34" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>136</v>
       </c>
@@ -2118,8 +2128,11 @@
       <c r="D35" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>140</v>
       </c>
@@ -2132,8 +2145,11 @@
       <c r="D36" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>144</v>
       </c>
@@ -2146,8 +2162,11 @@
       <c r="D37" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>148</v>
       </c>
@@ -2160,8 +2179,11 @@
       <c r="D38" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>152</v>
       </c>
@@ -2174,8 +2196,11 @@
       <c r="D39" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>156</v>
       </c>
@@ -2188,8 +2213,11 @@
       <c r="D40" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E40" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>160</v>
       </c>
@@ -2202,8 +2230,11 @@
       <c r="D41" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>164</v>
       </c>
@@ -2216,8 +2247,11 @@
       <c r="D42" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>168</v>
       </c>
@@ -2230,8 +2264,11 @@
       <c r="D43" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>172</v>
       </c>
@@ -2244,8 +2281,11 @@
       <c r="D44" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>176</v>
       </c>
@@ -2258,8 +2298,11 @@
       <c r="D45" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>180</v>
       </c>
@@ -2272,8 +2315,11 @@
       <c r="D46" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>184</v>
       </c>
@@ -2286,8 +2332,11 @@
       <c r="D47" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>188</v>
       </c>
@@ -2300,8 +2349,11 @@
       <c r="D48" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>192</v>
       </c>
@@ -2314,8 +2366,11 @@
       <c r="D49" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>196</v>
       </c>
@@ -2328,8 +2383,11 @@
       <c r="D50" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="E50" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>200</v>
       </c>
@@ -2342,8 +2400,11 @@
       <c r="D51" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>204</v>
       </c>
@@ -2356,8 +2417,11 @@
       <c r="D52" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>208</v>
       </c>
@@ -2370,8 +2434,11 @@
       <c r="D53" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>212</v>
       </c>
@@ -2384,8 +2451,11 @@
       <c r="D54" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>216</v>
       </c>
@@ -2400,6 +2470,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>